<commit_message>
Update attendance report: Y3_B2526_GIT_&_Liver_session_analysis.xlsx
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Session Analysis Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Session Analysis Results" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -52,8 +52,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFB6C1"/>
-        <bgColor rgb="00FFB6C1"/>
+        <fgColor rgb="0090EE90"/>
+        <bgColor rgb="0090EE90"/>
       </patternFill>
     </fill>
     <fill>
@@ -64,8 +64,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0090EE90"/>
-        <bgColor rgb="0090EE90"/>
+        <fgColor rgb="00FFB6C1"/>
+        <bgColor rgb="00FFB6C1"/>
       </patternFill>
     </fill>
   </fills>
@@ -81,7 +81,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -96,13 +96,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -484,7 +487,7 @@
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="13" customWidth="1" min="7" max="7"/>
+    <col width="50" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
     <col width="14" customWidth="1" min="9" max="9"/>
     <col width="22" customWidth="1" min="11" max="11"/>
@@ -576,15 +579,19 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr"/>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>mennatulla.medhat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>0/203</t>
+          <t>172/203</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
       <c r="K2" s="3" t="inlineStr">
@@ -796,7 +803,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -847,7 +854,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -898,7 +905,7 @@
         </is>
       </c>
       <c r="L8" s="5" t="n">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9">
@@ -932,15 +939,19 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G9" s="2" t="inlineStr"/>
+      <c r="G9" s="2" t="inlineStr">
+        <is>
+          <t>wessam.atef@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H9" s="2" t="inlineStr">
         <is>
-          <t>0/203</t>
+          <t>171/203</t>
         </is>
       </c>
       <c r="I9" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
       <c r="K9" s="5" t="inlineStr">
@@ -950,7 +961,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>6.5%</t>
         </is>
       </c>
     </row>
@@ -1003,7 +1014,7 @@
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>45.0%</t>
         </is>
       </c>
     </row>
@@ -1288,22 +1299,22 @@
         <v>31</v>
       </c>
       <c r="O15" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="P15" s="5" t="n">
         <v>0</v>
-      </c>
-      <c r="P15" s="5" t="n">
-        <v>2</v>
       </c>
       <c r="Q15" s="5" t="n">
         <v>29</v>
       </c>
       <c r="R15" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>6.5%</t>
         </is>
       </c>
       <c r="S15" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>84.5%</t>
         </is>
       </c>
     </row>
@@ -1366,22 +1377,22 @@
         <v>31</v>
       </c>
       <c r="O16" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="P16" s="5" t="n">
         <v>0</v>
-      </c>
-      <c r="P16" s="5" t="n">
-        <v>2</v>
       </c>
       <c r="Q16" s="5" t="n">
         <v>29</v>
       </c>
       <c r="R16" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>6.5%</t>
         </is>
       </c>
       <c r="S16" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>79.5%</t>
         </is>
       </c>
     </row>
@@ -1444,22 +1455,22 @@
         <v>31</v>
       </c>
       <c r="O17" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P17" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="5" t="n">
         <v>28</v>
       </c>
       <c r="R17" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>6.5%</t>
         </is>
       </c>
       <c r="S17" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>22.4%</t>
         </is>
       </c>
     </row>
@@ -1522,22 +1533,22 @@
         <v>31</v>
       </c>
       <c r="O18" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="P18" s="5" t="n">
         <v>0</v>
-      </c>
-      <c r="P18" s="5" t="n">
-        <v>2</v>
       </c>
       <c r="Q18" s="5" t="n">
         <v>29</v>
       </c>
       <c r="R18" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>6.5%</t>
         </is>
       </c>
       <c r="S18" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>11.4%</t>
         </is>
       </c>
     </row>
@@ -1600,22 +1611,22 @@
         <v>31</v>
       </c>
       <c r="O19" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="P19" s="5" t="n">
         <v>0</v>
-      </c>
-      <c r="P19" s="5" t="n">
-        <v>2</v>
       </c>
       <c r="Q19" s="5" t="n">
         <v>29</v>
       </c>
       <c r="R19" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>6.5%</t>
         </is>
       </c>
       <c r="S19" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>37.4%</t>
         </is>
       </c>
     </row>
@@ -1678,22 +1689,22 @@
         <v>31</v>
       </c>
       <c r="O20" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P20" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="5" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R20" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>6.5%</t>
         </is>
       </c>
       <c r="S20" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>34.9%</t>
         </is>
       </c>
     </row>
@@ -2309,15 +2320,19 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G33" s="2" t="inlineStr"/>
+      <c r="G33" s="2" t="inlineStr">
+        <is>
+          <t>mennatulla.medhat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H33" s="2" t="inlineStr">
         <is>
-          <t>0/205</t>
+          <t>162/205</t>
         </is>
       </c>
       <c r="I33" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -2610,15 +2625,19 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G40" s="2" t="inlineStr"/>
+      <c r="G40" s="2" t="inlineStr">
+        <is>
+          <t>wessam.atef@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H40" s="2" t="inlineStr">
         <is>
-          <t>0/205</t>
+          <t>164/205</t>
         </is>
       </c>
       <c r="I40" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -3642,56 +3661,60 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G64" s="2" t="inlineStr"/>
+      <c r="G64" s="2" t="inlineStr">
+        <is>
+          <t>mennatulla.medhat@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
+          <t>24/221</t>
+        </is>
+      </c>
+      <c r="I64" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="9" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B65" s="9" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+      <c r="C65" s="9" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="D65" s="9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E65" s="9" t="inlineStr">
+        <is>
+          <t>28/09/2025</t>
+        </is>
+      </c>
+      <c r="F65" s="9" t="inlineStr">
+        <is>
+          <t>08:00:00</t>
+        </is>
+      </c>
+      <c r="G65" s="9" t="inlineStr"/>
+      <c r="H65" s="9" t="inlineStr">
+        <is>
           <t>0/221</t>
         </is>
       </c>
-      <c r="I64" s="2" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="2" t="inlineStr">
-        <is>
-          <t>Year 3</t>
-        </is>
-      </c>
-      <c r="B65" s="2" t="inlineStr">
-        <is>
-          <t>A3</t>
-        </is>
-      </c>
-      <c r="C65" s="2" t="inlineStr">
-        <is>
-          <t>ANATOMY</t>
-        </is>
-      </c>
-      <c r="D65" s="2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E65" s="2" t="inlineStr">
-        <is>
-          <t>28/09/2025</t>
-        </is>
-      </c>
-      <c r="F65" s="2" t="inlineStr">
-        <is>
-          <t>08:00:00</t>
-        </is>
-      </c>
-      <c r="G65" s="2" t="inlineStr"/>
-      <c r="H65" s="2" t="inlineStr">
-        <is>
-          <t>0/221</t>
-        </is>
-      </c>
-      <c r="I65" s="2" t="inlineStr">
+      <c r="I65" s="9" t="inlineStr">
         <is>
           <t>Not Recorded</t>
         </is>
@@ -3943,15 +3966,19 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G71" s="2" t="inlineStr"/>
+      <c r="G71" s="2" t="inlineStr">
+        <is>
+          <t>Omnia.Mohammed@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H71" s="2" t="inlineStr">
         <is>
-          <t>0/221</t>
+          <t>75/221</t>
         </is>
       </c>
       <c r="I71" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -4975,15 +5002,19 @@
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G95" s="2" t="inlineStr"/>
+      <c r="G95" s="2" t="inlineStr">
+        <is>
+          <t>mennatulla.medhat@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H95" s="2" t="inlineStr">
         <is>
-          <t>0/132</t>
+          <t>2/132</t>
         </is>
       </c>
       <c r="I95" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -5276,15 +5307,19 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G102" s="2" t="inlineStr"/>
+      <c r="G102" s="2" t="inlineStr">
+        <is>
+          <t>aml.awwad@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H102" s="2" t="inlineStr">
         <is>
-          <t>0/132</t>
+          <t>28/132</t>
         </is>
       </c>
       <c r="I102" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -6308,15 +6343,19 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G126" s="2" t="inlineStr"/>
+      <c r="G126" s="2" t="inlineStr">
+        <is>
+          <t>mennatulla.medhat@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H126" s="2" t="inlineStr">
         <is>
-          <t>0/230</t>
+          <t>67/230</t>
         </is>
       </c>
       <c r="I126" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -6609,15 +6648,19 @@
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G133" s="2" t="inlineStr"/>
+      <c r="G133" s="2" t="inlineStr">
+        <is>
+          <t>aml.awwad@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H133" s="2" t="inlineStr">
         <is>
-          <t>0/230</t>
+          <t>105/230</t>
         </is>
       </c>
       <c r="I133" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -7641,58 +7684,62 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G157" s="2" t="inlineStr"/>
+      <c r="G157" s="2" t="inlineStr">
+        <is>
+          <t>majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H157" s="2" t="inlineStr">
         <is>
+          <t>69/222</t>
+        </is>
+      </c>
+      <c r="I157" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="9" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B158" s="9" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C158" s="9" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="D158" s="9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E158" s="9" t="inlineStr">
+        <is>
+          <t>28/09/2025</t>
+        </is>
+      </c>
+      <c r="F158" s="9" t="inlineStr">
+        <is>
+          <t>10:00:00</t>
+        </is>
+      </c>
+      <c r="G158" s="9" t="inlineStr"/>
+      <c r="H158" s="9" t="inlineStr">
+        <is>
           <t>0/222</t>
         </is>
       </c>
-      <c r="I157" s="2" t="inlineStr">
+      <c r="I158" s="9" t="inlineStr">
         <is>
           <t>Not Recorded</t>
-        </is>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" s="4" t="inlineStr">
-        <is>
-          <t>Year 3</t>
-        </is>
-      </c>
-      <c r="B158" s="4" t="inlineStr">
-        <is>
-          <t>B3</t>
-        </is>
-      </c>
-      <c r="C158" s="4" t="inlineStr">
-        <is>
-          <t>ANATOMY</t>
-        </is>
-      </c>
-      <c r="D158" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E158" s="4" t="inlineStr">
-        <is>
-          <t>28/09/2025</t>
-        </is>
-      </c>
-      <c r="F158" s="4" t="inlineStr">
-        <is>
-          <t>10:00:00</t>
-        </is>
-      </c>
-      <c r="G158" s="4" t="inlineStr"/>
-      <c r="H158" s="4" t="inlineStr">
-        <is>
-          <t>0/222</t>
-        </is>
-      </c>
-      <c r="I158" s="4" t="inlineStr">
-        <is>
-          <t>Pending</t>
         </is>
       </c>
     </row>
@@ -7942,15 +7989,19 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G164" s="2" t="inlineStr"/>
+      <c r="G164" s="2" t="inlineStr">
+        <is>
+          <t>Omnia.Mohammed@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H164" s="2" t="inlineStr">
         <is>
-          <t>0/222</t>
+          <t>86/222</t>
         </is>
       </c>
       <c r="I164" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2025-09-28 09:21:19
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Session Analysis Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Session Analysis Results" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -52,8 +52,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0090EE90"/>
-        <bgColor rgb="0090EE90"/>
+        <fgColor rgb="00FFB6C1"/>
+        <bgColor rgb="00FFB6C1"/>
       </patternFill>
     </fill>
     <fill>
@@ -64,8 +64,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFB6C1"/>
-        <bgColor rgb="00FFB6C1"/>
+        <fgColor rgb="0090EE90"/>
+        <bgColor rgb="0090EE90"/>
       </patternFill>
     </fill>
   </fills>
@@ -81,7 +81,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -96,16 +96,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -487,7 +484,7 @@
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="50" customWidth="1" min="7" max="7"/>
+    <col width="13" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
     <col width="14" customWidth="1" min="9" max="9"/>
     <col width="22" customWidth="1" min="11" max="11"/>
@@ -579,19 +576,15 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>mennatulla.medhat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
-        </is>
-      </c>
+      <c r="G2" s="2" t="inlineStr"/>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>172/203</t>
+          <t>0/203</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>Recorded</t>
+          <t>Not Recorded</t>
         </is>
       </c>
       <c r="K2" s="3" t="inlineStr">
@@ -803,7 +796,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -854,7 +847,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -905,7 +898,7 @@
         </is>
       </c>
       <c r="L8" s="5" t="n">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9">
@@ -939,19 +932,15 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G9" s="2" t="inlineStr">
-        <is>
-          <t>wessam.atef@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg</t>
-        </is>
-      </c>
+      <c r="G9" s="2" t="inlineStr"/>
       <c r="H9" s="2" t="inlineStr">
         <is>
-          <t>171/203</t>
+          <t>0/203</t>
         </is>
       </c>
       <c r="I9" s="2" t="inlineStr">
         <is>
-          <t>Recorded</t>
+          <t>Not Recorded</t>
         </is>
       </c>
       <c r="K9" s="5" t="inlineStr">
@@ -961,7 +950,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>6.5%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -1014,7 +1003,7 @@
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>45.0%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -1299,22 +1288,22 @@
         <v>31</v>
       </c>
       <c r="O15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" s="5" t="n">
         <v>2</v>
-      </c>
-      <c r="P15" s="5" t="n">
-        <v>0</v>
       </c>
       <c r="Q15" s="5" t="n">
         <v>29</v>
       </c>
       <c r="R15" s="5" t="inlineStr">
         <is>
-          <t>6.5%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="S15" s="5" t="inlineStr">
         <is>
-          <t>84.5%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -1377,22 +1366,22 @@
         <v>31</v>
       </c>
       <c r="O16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" s="5" t="n">
         <v>2</v>
-      </c>
-      <c r="P16" s="5" t="n">
-        <v>0</v>
       </c>
       <c r="Q16" s="5" t="n">
         <v>29</v>
       </c>
       <c r="R16" s="5" t="inlineStr">
         <is>
-          <t>6.5%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="S16" s="5" t="inlineStr">
         <is>
-          <t>79.5%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -1455,22 +1444,22 @@
         <v>31</v>
       </c>
       <c r="O17" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P17" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q17" s="5" t="n">
         <v>28</v>
       </c>
       <c r="R17" s="5" t="inlineStr">
         <is>
-          <t>6.5%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="S17" s="5" t="inlineStr">
         <is>
-          <t>22.4%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -1533,22 +1522,22 @@
         <v>31</v>
       </c>
       <c r="O18" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" s="5" t="n">
         <v>2</v>
-      </c>
-      <c r="P18" s="5" t="n">
-        <v>0</v>
       </c>
       <c r="Q18" s="5" t="n">
         <v>29</v>
       </c>
       <c r="R18" s="5" t="inlineStr">
         <is>
-          <t>6.5%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="S18" s="5" t="inlineStr">
         <is>
-          <t>11.4%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -1611,22 +1600,22 @@
         <v>31</v>
       </c>
       <c r="O19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" s="5" t="n">
         <v>2</v>
-      </c>
-      <c r="P19" s="5" t="n">
-        <v>0</v>
       </c>
       <c r="Q19" s="5" t="n">
         <v>29</v>
       </c>
       <c r="R19" s="5" t="inlineStr">
         <is>
-          <t>6.5%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="S19" s="5" t="inlineStr">
         <is>
-          <t>37.4%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -1689,22 +1678,22 @@
         <v>31</v>
       </c>
       <c r="O20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="P20" s="5" t="n">
-        <v>1</v>
-      </c>
       <c r="Q20" s="5" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R20" s="5" t="inlineStr">
         <is>
-          <t>6.5%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="S20" s="5" t="inlineStr">
         <is>
-          <t>34.9%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -2320,19 +2309,15 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G33" s="2" t="inlineStr">
-        <is>
-          <t>mennatulla.medhat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
-        </is>
-      </c>
+      <c r="G33" s="2" t="inlineStr"/>
       <c r="H33" s="2" t="inlineStr">
         <is>
-          <t>162/205</t>
+          <t>0/205</t>
         </is>
       </c>
       <c r="I33" s="2" t="inlineStr">
         <is>
-          <t>Recorded</t>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -2625,19 +2610,15 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G40" s="2" t="inlineStr">
-        <is>
-          <t>wessam.atef@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg</t>
-        </is>
-      </c>
+      <c r="G40" s="2" t="inlineStr"/>
       <c r="H40" s="2" t="inlineStr">
         <is>
-          <t>164/205</t>
+          <t>0/205</t>
         </is>
       </c>
       <c r="I40" s="2" t="inlineStr">
         <is>
-          <t>Recorded</t>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -3661,60 +3642,56 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G64" s="2" t="inlineStr">
-        <is>
-          <t>mennatulla.medhat@med.asu.edu.eg</t>
-        </is>
-      </c>
+      <c r="G64" s="2" t="inlineStr"/>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>24/221</t>
+          <t>0/221</t>
         </is>
       </c>
       <c r="I64" s="2" t="inlineStr">
         <is>
-          <t>Recorded</t>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="9" t="inlineStr">
-        <is>
-          <t>Year 3</t>
-        </is>
-      </c>
-      <c r="B65" s="9" t="inlineStr">
+      <c r="A65" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B65" s="2" t="inlineStr">
         <is>
           <t>A3</t>
         </is>
       </c>
-      <c r="C65" s="9" t="inlineStr">
+      <c r="C65" s="2" t="inlineStr">
         <is>
           <t>ANATOMY</t>
         </is>
       </c>
-      <c r="D65" s="9" t="inlineStr">
+      <c r="D65" s="2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E65" s="9" t="inlineStr">
+      <c r="E65" s="2" t="inlineStr">
         <is>
           <t>28/09/2025</t>
         </is>
       </c>
-      <c r="F65" s="9" t="inlineStr">
+      <c r="F65" s="2" t="inlineStr">
         <is>
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G65" s="9" t="inlineStr"/>
-      <c r="H65" s="9" t="inlineStr">
+      <c r="G65" s="2" t="inlineStr"/>
+      <c r="H65" s="2" t="inlineStr">
         <is>
           <t>0/221</t>
         </is>
       </c>
-      <c r="I65" s="9" t="inlineStr">
+      <c r="I65" s="2" t="inlineStr">
         <is>
           <t>Not Recorded</t>
         </is>
@@ -3966,19 +3943,15 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G71" s="2" t="inlineStr">
-        <is>
-          <t>Omnia.Mohammed@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
-        </is>
-      </c>
+      <c r="G71" s="2" t="inlineStr"/>
       <c r="H71" s="2" t="inlineStr">
         <is>
-          <t>75/221</t>
+          <t>0/221</t>
         </is>
       </c>
       <c r="I71" s="2" t="inlineStr">
         <is>
-          <t>Recorded</t>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -5002,19 +4975,15 @@
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G95" s="2" t="inlineStr">
-        <is>
-          <t>mennatulla.medhat@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
-        </is>
-      </c>
+      <c r="G95" s="2" t="inlineStr"/>
       <c r="H95" s="2" t="inlineStr">
         <is>
-          <t>2/132</t>
+          <t>0/132</t>
         </is>
       </c>
       <c r="I95" s="2" t="inlineStr">
         <is>
-          <t>Recorded</t>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -5307,19 +5276,15 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G102" s="2" t="inlineStr">
-        <is>
-          <t>aml.awwad@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
-        </is>
-      </c>
+      <c r="G102" s="2" t="inlineStr"/>
       <c r="H102" s="2" t="inlineStr">
         <is>
-          <t>28/132</t>
+          <t>0/132</t>
         </is>
       </c>
       <c r="I102" s="2" t="inlineStr">
         <is>
-          <t>Recorded</t>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -6343,19 +6308,15 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G126" s="2" t="inlineStr">
-        <is>
-          <t>mennatulla.medhat@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
-        </is>
-      </c>
+      <c r="G126" s="2" t="inlineStr"/>
       <c r="H126" s="2" t="inlineStr">
         <is>
-          <t>67/230</t>
+          <t>0/230</t>
         </is>
       </c>
       <c r="I126" s="2" t="inlineStr">
         <is>
-          <t>Recorded</t>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -6648,19 +6609,15 @@
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G133" s="2" t="inlineStr">
-        <is>
-          <t>aml.awwad@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
-        </is>
-      </c>
+      <c r="G133" s="2" t="inlineStr"/>
       <c r="H133" s="2" t="inlineStr">
         <is>
-          <t>105/230</t>
+          <t>0/230</t>
         </is>
       </c>
       <c r="I133" s="2" t="inlineStr">
         <is>
-          <t>Recorded</t>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -7684,62 +7641,58 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G157" s="2" t="inlineStr">
-        <is>
-          <t>majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
-        </is>
-      </c>
+      <c r="G157" s="2" t="inlineStr"/>
       <c r="H157" s="2" t="inlineStr">
         <is>
-          <t>69/222</t>
+          <t>0/222</t>
         </is>
       </c>
       <c r="I157" s="2" t="inlineStr">
         <is>
-          <t>Recorded</t>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="9" t="inlineStr">
-        <is>
-          <t>Year 3</t>
-        </is>
-      </c>
-      <c r="B158" s="9" t="inlineStr">
+      <c r="A158" s="4" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B158" s="4" t="inlineStr">
         <is>
           <t>B3</t>
         </is>
       </c>
-      <c r="C158" s="9" t="inlineStr">
+      <c r="C158" s="4" t="inlineStr">
         <is>
           <t>ANATOMY</t>
         </is>
       </c>
-      <c r="D158" s="9" t="inlineStr">
+      <c r="D158" s="4" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E158" s="9" t="inlineStr">
+      <c r="E158" s="4" t="inlineStr">
         <is>
           <t>28/09/2025</t>
         </is>
       </c>
-      <c r="F158" s="9" t="inlineStr">
+      <c r="F158" s="4" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G158" s="9" t="inlineStr"/>
-      <c r="H158" s="9" t="inlineStr">
+      <c r="G158" s="4" t="inlineStr"/>
+      <c r="H158" s="4" t="inlineStr">
         <is>
           <t>0/222</t>
         </is>
       </c>
-      <c r="I158" s="9" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="I158" s="4" t="inlineStr">
+        <is>
+          <t>Pending</t>
         </is>
       </c>
     </row>
@@ -7989,19 +7942,15 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G164" s="2" t="inlineStr">
-        <is>
-          <t>Omnia.Mohammed@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
-        </is>
-      </c>
+      <c r="G164" s="2" t="inlineStr"/>
       <c r="H164" s="2" t="inlineStr">
         <is>
-          <t>86/222</t>
+          <t>0/222</t>
         </is>
       </c>
       <c r="I164" s="2" t="inlineStr">
         <is>
-          <t>Recorded</t>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2025-09-28 13:24:34
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
@@ -898,7 +898,7 @@
         </is>
       </c>
       <c r="L8" s="5" t="n">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9">
@@ -1681,10 +1681,10 @@
         <v>0</v>
       </c>
       <c r="P20" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q20" s="5" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R20" s="5" t="inlineStr">
         <is>
@@ -7654,45 +7654,45 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="4" t="inlineStr">
-        <is>
-          <t>Year 3</t>
-        </is>
-      </c>
-      <c r="B158" s="4" t="inlineStr">
+      <c r="A158" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B158" s="2" t="inlineStr">
         <is>
           <t>B3</t>
         </is>
       </c>
-      <c r="C158" s="4" t="inlineStr">
+      <c r="C158" s="2" t="inlineStr">
         <is>
           <t>ANATOMY</t>
         </is>
       </c>
-      <c r="D158" s="4" t="inlineStr">
+      <c r="D158" s="2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E158" s="4" t="inlineStr">
+      <c r="E158" s="2" t="inlineStr">
         <is>
           <t>28/09/2025</t>
         </is>
       </c>
-      <c r="F158" s="4" t="inlineStr">
+      <c r="F158" s="2" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G158" s="4" t="inlineStr"/>
-      <c r="H158" s="4" t="inlineStr">
+      <c r="G158" s="2" t="inlineStr"/>
+      <c r="H158" s="2" t="inlineStr">
         <is>
           <t>0/222</t>
         </is>
       </c>
-      <c r="I158" s="4" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="I158" s="2" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2025-09-28 15:16:18
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -52,8 +52,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFB6C1"/>
-        <bgColor rgb="00FFB6C1"/>
+        <fgColor rgb="0090EE90"/>
+        <bgColor rgb="0090EE90"/>
       </patternFill>
     </fill>
     <fill>
@@ -64,8 +64,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0090EE90"/>
-        <bgColor rgb="0090EE90"/>
+        <fgColor rgb="00FFB6C1"/>
+        <bgColor rgb="00FFB6C1"/>
       </patternFill>
     </fill>
   </fills>
@@ -96,10 +96,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -484,9 +484,9 @@
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="13" customWidth="1" min="7" max="7"/>
+    <col width="50" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
-    <col width="14" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
     <col width="22" customWidth="1" min="11" max="11"/>
     <col width="8" customWidth="1" min="12" max="12"/>
     <col width="18" customWidth="1" min="13" max="13"/>
@@ -576,15 +576,19 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr"/>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>mennatulla.medhat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>0/203</t>
+          <t>172/203</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
       <c r="K2" s="3" t="inlineStr">
@@ -796,7 +800,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
@@ -847,7 +851,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -932,15 +936,19 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G9" s="2" t="inlineStr"/>
+      <c r="G9" s="2" t="inlineStr">
+        <is>
+          <t>Safa.hany@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg, wessam.atef@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H9" s="2" t="inlineStr">
         <is>
-          <t>0/203</t>
+          <t>168/203</t>
         </is>
       </c>
       <c r="I9" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
       <c r="K9" s="5" t="inlineStr">
@@ -950,7 +958,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>7.5%</t>
         </is>
       </c>
     </row>
@@ -1003,7 +1011,7 @@
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>42.0%</t>
         </is>
       </c>
     </row>
@@ -1288,22 +1296,22 @@
         <v>31</v>
       </c>
       <c r="O15" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="P15" s="5" t="n">
         <v>0</v>
-      </c>
-      <c r="P15" s="5" t="n">
-        <v>2</v>
       </c>
       <c r="Q15" s="5" t="n">
         <v>29</v>
       </c>
       <c r="R15" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>6.5%</t>
         </is>
       </c>
       <c r="S15" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>83.7%</t>
         </is>
       </c>
     </row>
@@ -1366,22 +1374,22 @@
         <v>31</v>
       </c>
       <c r="O16" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="P16" s="5" t="n">
         <v>0</v>
-      </c>
-      <c r="P16" s="5" t="n">
-        <v>2</v>
       </c>
       <c r="Q16" s="5" t="n">
         <v>29</v>
       </c>
       <c r="R16" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>6.5%</t>
         </is>
       </c>
       <c r="S16" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>79.5%</t>
         </is>
       </c>
     </row>
@@ -1444,22 +1452,22 @@
         <v>31</v>
       </c>
       <c r="O17" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="P17" s="5" t="n">
         <v>0</v>
-      </c>
-      <c r="P17" s="5" t="n">
-        <v>3</v>
       </c>
       <c r="Q17" s="5" t="n">
         <v>28</v>
       </c>
       <c r="R17" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>9.7%</t>
         </is>
       </c>
       <c r="S17" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>27.3%</t>
         </is>
       </c>
     </row>
@@ -1522,22 +1530,22 @@
         <v>31</v>
       </c>
       <c r="O18" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="P18" s="5" t="n">
         <v>0</v>
-      </c>
-      <c r="P18" s="5" t="n">
-        <v>2</v>
       </c>
       <c r="Q18" s="5" t="n">
         <v>29</v>
       </c>
       <c r="R18" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>6.5%</t>
         </is>
       </c>
       <c r="S18" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>11.4%</t>
         </is>
       </c>
     </row>
@@ -1600,22 +1608,22 @@
         <v>31</v>
       </c>
       <c r="O19" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="P19" s="5" t="n">
         <v>0</v>
-      </c>
-      <c r="P19" s="5" t="n">
-        <v>2</v>
       </c>
       <c r="Q19" s="5" t="n">
         <v>29</v>
       </c>
       <c r="R19" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>6.5%</t>
         </is>
       </c>
       <c r="S19" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>30.2%</t>
         </is>
       </c>
     </row>
@@ -1678,22 +1686,22 @@
         <v>31</v>
       </c>
       <c r="O20" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="P20" s="5" t="n">
         <v>0</v>
-      </c>
-      <c r="P20" s="5" t="n">
-        <v>3</v>
       </c>
       <c r="Q20" s="5" t="n">
         <v>28</v>
       </c>
       <c r="R20" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>9.7%</t>
         </is>
       </c>
       <c r="S20" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>32.1%</t>
         </is>
       </c>
     </row>
@@ -2309,15 +2317,19 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G33" s="2" t="inlineStr"/>
+      <c r="G33" s="2" t="inlineStr">
+        <is>
+          <t>mennatulla.medhat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H33" s="2" t="inlineStr">
         <is>
-          <t>0/205</t>
+          <t>162/205</t>
         </is>
       </c>
       <c r="I33" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -2610,15 +2622,19 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G40" s="2" t="inlineStr"/>
+      <c r="G40" s="2" t="inlineStr">
+        <is>
+          <t>Safa.hany@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg, wessam.atef@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H40" s="2" t="inlineStr">
         <is>
-          <t>0/205</t>
+          <t>164/205</t>
         </is>
       </c>
       <c r="I40" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -3642,15 +3658,19 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G64" s="2" t="inlineStr"/>
+      <c r="G64" s="2" t="inlineStr">
+        <is>
+          <t>mennatulla.medhat@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>0/221</t>
+          <t>39/221</t>
         </is>
       </c>
       <c r="I64" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -3685,15 +3705,19 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G65" s="2" t="inlineStr"/>
+      <c r="G65" s="2" t="inlineStr">
+        <is>
+          <t>mennatulla.medhat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H65" s="2" t="inlineStr">
         <is>
-          <t>0/221</t>
+          <t>63/221</t>
         </is>
       </c>
       <c r="I65" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -3943,15 +3967,19 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G71" s="2" t="inlineStr"/>
+      <c r="G71" s="2" t="inlineStr">
+        <is>
+          <t>Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H71" s="2" t="inlineStr">
         <is>
-          <t>0/221</t>
+          <t>79/221</t>
         </is>
       </c>
       <c r="I71" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -4975,15 +5003,19 @@
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G95" s="2" t="inlineStr"/>
+      <c r="G95" s="2" t="inlineStr">
+        <is>
+          <t>Veronia.rafat@med.asu.edu.eg, mennatulla.medhat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H95" s="2" t="inlineStr">
         <is>
-          <t>0/132</t>
+          <t>2/132</t>
         </is>
       </c>
       <c r="I95" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -5276,15 +5308,19 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G102" s="2" t="inlineStr"/>
+      <c r="G102" s="2" t="inlineStr">
+        <is>
+          <t>aml.awwad@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H102" s="2" t="inlineStr">
         <is>
-          <t>0/132</t>
+          <t>28/132</t>
         </is>
       </c>
       <c r="I102" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -6308,15 +6344,19 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G126" s="2" t="inlineStr"/>
+      <c r="G126" s="2" t="inlineStr">
+        <is>
+          <t>Veronia.rafat@med.asu.edu.eg, mennatulla.medhat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H126" s="2" t="inlineStr">
         <is>
-          <t>0/230</t>
+          <t>33/230</t>
         </is>
       </c>
       <c r="I126" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -6609,15 +6649,19 @@
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G133" s="2" t="inlineStr"/>
+      <c r="G133" s="2" t="inlineStr">
+        <is>
+          <t>aml.awwad@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H133" s="2" t="inlineStr">
         <is>
-          <t>0/230</t>
+          <t>106/230</t>
         </is>
       </c>
       <c r="I133" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -7641,15 +7685,19 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G157" s="2" t="inlineStr"/>
+      <c r="G157" s="2" t="inlineStr">
+        <is>
+          <t>servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H157" s="2" t="inlineStr">
         <is>
-          <t>0/222</t>
+          <t>69/222</t>
         </is>
       </c>
       <c r="I157" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -7684,15 +7732,19 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G158" s="2" t="inlineStr"/>
+      <c r="G158" s="2" t="inlineStr">
+        <is>
+          <t>mennatulla.medhat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H158" s="2" t="inlineStr">
         <is>
-          <t>0/222</t>
+          <t>59/222</t>
         </is>
       </c>
       <c r="I158" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -7942,15 +7994,19 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G164" s="2" t="inlineStr"/>
+      <c r="G164" s="2" t="inlineStr">
+        <is>
+          <t>Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H164" s="2" t="inlineStr">
         <is>
-          <t>0/222</t>
+          <t>86/222</t>
         </is>
       </c>
       <c r="I164" s="2" t="inlineStr">
         <is>
-          <t>Not Recorded</t>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2025-09-29 03:39:41
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -938,7 +938,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg, wessam.atef@med.asu.edu.eg</t>
+          <t>Sara_nabil@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, wessam.atef@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -2624,7 +2624,7 @@
       </c>
       <c r="G40" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg, wessam.atef@med.asu.edu.eg</t>
+          <t>Sara_nabil@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, wessam.atef@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H40" s="2" t="inlineStr">
@@ -3969,7 +3969,7 @@
       </c>
       <c r="G71" s="2" t="inlineStr">
         <is>
-          <t>Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+          <t>Sara_nabil@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H71" s="2" t="inlineStr">
@@ -5005,7 +5005,7 @@
       </c>
       <c r="G95" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, mennatulla.medhat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, mennatulla.medhat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H95" s="2" t="inlineStr">
@@ -5310,7 +5310,7 @@
       </c>
       <c r="G102" s="2" t="inlineStr">
         <is>
-          <t>aml.awwad@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+          <t>mariam.noureldin@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg, aml.awwad@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H102" s="2" t="inlineStr">
@@ -6346,7 +6346,7 @@
       </c>
       <c r="G126" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, mennatulla.medhat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, mennatulla.medhat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H126" s="2" t="inlineStr">
@@ -6651,7 +6651,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>aml.awwad@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+          <t>mariam.noureldin@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg, aml.awwad@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7687,7 +7687,7 @@
       </c>
       <c r="G157" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H157" s="2" t="inlineStr">
@@ -7996,7 +7996,7 @@
       </c>
       <c r="G164" s="2" t="inlineStr">
         <is>
-          <t>Omnia.Mohammed@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+          <t>Sara_nabil@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H164" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2025-09-29 20:56:56
</commit_message>
<xml_diff>
--- a/attendance_reports/Y3_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y3_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -938,7 +938,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>wessam.atef@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg</t>
+          <t>wessam.atef@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="G29" s="2" t="inlineStr">
         <is>
-          <t>aya.hanafy@med.asu.edu.eg, marinasorial@med.asu.edu.eg, yasmin.m.senosy@med.asu.edu.eg, shorokmohamed@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, ola.m.abdelfattah@med.asu.edu.eg, Remon.Matta@med.asu.edu.eg, nardine.alfonse@med.asu.edu.eg</t>
+          <t>neveen.nashaat@med.asu.edu.eg, aya.hanafy@med.asu.edu.eg, shorokmohamed@med.asu.edu.eg, ola.m.abdelfattah@med.asu.edu.eg, yasmin.m.senosy@med.asu.edu.eg, marinasorial@med.asu.edu.eg, nardine.alfonse@med.asu.edu.eg, Remon.Matta@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H29" s="2" t="inlineStr">
@@ -2628,7 +2628,7 @@
       </c>
       <c r="G40" s="2" t="inlineStr">
         <is>
-          <t>wessam.atef@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg</t>
+          <t>wessam.atef@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H40" s="2" t="inlineStr">
@@ -3492,7 +3492,7 @@
       </c>
       <c r="G60" s="2" t="inlineStr">
         <is>
-          <t>aya.hanafy@med.asu.edu.eg, marinasorial@med.asu.edu.eg, yasmin.m.senosy@med.asu.edu.eg, shorokmohamed@med.asu.edu.eg, neveen.nashaat@med.asu.edu.eg, ola.m.abdelfattah@med.asu.edu.eg, Remon.Matta@med.asu.edu.eg, nardine.alfonse@med.asu.edu.eg</t>
+          <t>neveen.nashaat@med.asu.edu.eg, aya.hanafy@med.asu.edu.eg, shorokmohamed@med.asu.edu.eg, ola.m.abdelfattah@med.asu.edu.eg, yasmin.m.senosy@med.asu.edu.eg, marinasorial@med.asu.edu.eg, nardine.alfonse@med.asu.edu.eg, Remon.Matta@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H60" s="2" t="inlineStr">
@@ -3715,7 +3715,7 @@
       </c>
       <c r="G65" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, mennatulla.medhat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>mennatulla.medhat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H65" s="2" t="inlineStr">
@@ -3977,7 +3977,7 @@
       </c>
       <c r="G71" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+          <t>Sara_nabil@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H71" s="2" t="inlineStr">
@@ -5318,7 +5318,7 @@
       </c>
       <c r="G102" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, aml.awwad@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg</t>
+          <t>aml.awwad@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H102" s="2" t="inlineStr">
@@ -6659,7 +6659,7 @@
       </c>
       <c r="G133" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, aml.awwad@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg</t>
+          <t>aml.awwad@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, norhan.mohamed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H133" s="2" t="inlineStr">
@@ -7695,7 +7695,7 @@
       </c>
       <c r="G157" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H157" s="2" t="inlineStr">
@@ -7742,7 +7742,7 @@
       </c>
       <c r="G158" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, mennatulla.medhat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>mennatulla.medhat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H158" s="2" t="inlineStr">
@@ -8004,7 +8004,7 @@
       </c>
       <c r="G164" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Sara_nabil@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg</t>
+          <t>Sara_nabil@med.asu.edu.eg, Safa.hany@med.asu.edu.eg, mariam.noureldin@med.asu.edu.eg, Omnia.Mohammed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H164" s="2" t="inlineStr">

</xml_diff>